<commit_message>
UPD : 12th May 2023
</commit_message>
<xml_diff>
--- a/IPL/Data/exp/pstats_v01_Gujarat Titans.xlsx
+++ b/IPL/Data/exp/pstats_v01_Gujarat Titans.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BS17"/>
+  <dimension ref="A1:BT17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,315 +476,320 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>lpos</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>batnum_min</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>tbf</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>tr_pp</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>tbf_pp</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>tout_pp</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>tr_mid</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>tbf_mid</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>tout_mid</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>tr_dth</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>tbf_dth</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>tout_dth</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>f.cp.pts30</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>f.cp.pts50</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>f.cp.pts100</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>f.cp.pts0</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>tbb</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>tbrc</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>tbov.powp</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>tbov.mid</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>tbov.dth</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>tbrc_powp</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>tbrc_mid</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>tbrc_dth</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>tbwkt_powp</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>tbwkt_mid</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>tbwkt_dth</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>bat_tm</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>bat</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>tr.G01</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>tr.G07</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>tr.G13</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>tr.G18</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>tr.G23</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>tr.G30</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>tr.G35</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>tr.G39</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>tr.G44</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>bow_tm</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>bow</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G01</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G07</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G13</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G18</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G23</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G30</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G35</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G39</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>tbwkt.G44</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>tr%.pp</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>tr%.mid</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>tr%.dth</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>tr</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>tinn</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>tbov%.pp</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>tbov%.mid</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>tbov%.dth</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>tbwkt%.pp</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>tbwkt%.mid</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>tbwkt%.dth</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>tbwkt</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>tbov</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>tr_tinn_ratio</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>4xtbwkt_tbov_ratio</t>
         </is>
@@ -798,12 +803,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A Manohar</t>
+          <t>WP Saha</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Abhinav Manohar</t>
+          <t>Wriddhiman Saha</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -811,64 +816,48 @@
           <t>RHB</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RALB</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Right</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Spin</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>leg-break</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="N2" t="n">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="O2" t="n">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="P2" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="Q2" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -877,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -909,36 +898,46 @@
       <c r="AH2" t="n">
         <v>0</v>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>A Manohar</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>WP Saha</t>
+        </is>
+      </c>
+      <c r="AL2" t="n">
+        <v>25</v>
+      </c>
       <c r="AM2" t="n">
         <v>14</v>
       </c>
-      <c r="AN2" t="inlineStr"/>
+      <c r="AN2" t="n">
+        <v>17</v>
+      </c>
       <c r="AO2" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AP2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ2" t="n">
-        <v>42</v>
-      </c>
-      <c r="AR2" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>4</v>
+      </c>
       <c r="AS2" t="n">
-        <v>26</v>
-      </c>
-      <c r="AT2" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0</v>
+      </c>
       <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr"/>
@@ -949,37 +948,38 @@
       <c r="BB2" t="inlineStr"/>
       <c r="BC2" t="inlineStr"/>
       <c r="BD2" t="inlineStr"/>
-      <c r="BE2" t="n">
-        <v>0</v>
-      </c>
+      <c r="BE2" t="inlineStr"/>
       <c r="BF2" t="n">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="BG2" t="n">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="BH2" t="n">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="BI2" t="n">
-        <v>5</v>
-      </c>
-      <c r="BJ2" t="inlineStr"/>
+        <v>151</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>9</v>
+      </c>
       <c r="BK2" t="inlineStr"/>
       <c r="BL2" t="inlineStr"/>
       <c r="BM2" t="inlineStr"/>
       <c r="BN2" t="inlineStr"/>
       <c r="BO2" t="inlineStr"/>
-      <c r="BP2" t="n">
-        <v>0</v>
-      </c>
+      <c r="BP2" t="inlineStr"/>
       <c r="BQ2" t="n">
         <v>0</v>
       </c>
       <c r="BR2" t="n">
-        <v>22.4</v>
-      </c>
-      <c r="BS2" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>17</v>
+      </c>
+      <c r="BT2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -989,12 +989,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AS Joseph</t>
+          <t>Shubman Gill</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Alzarri Joseph</t>
+          <t>Shubman Gill</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RAFM</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1014,169 +1014,174 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pace</t>
+          <t>Spin</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>fast-medium</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>off-break</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>114</v>
+        <v>-2</v>
       </c>
       <c r="Y3" t="n">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>Shubman Gill</t>
+        </is>
+      </c>
+      <c r="AL3" t="n">
+        <v>63</v>
+      </c>
+      <c r="AM3" t="n">
         <v>14</v>
       </c>
-      <c r="AF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>AS Joseph</t>
-        </is>
-      </c>
-      <c r="AV3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AN3" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>67</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>45</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>56</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>49</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
       <c r="BA3" t="inlineStr"/>
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
       <c r="BD3" t="inlineStr"/>
       <c r="BE3" t="inlineStr"/>
-      <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr"/>
+      <c r="BF3" t="n">
+        <v>49</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>47</v>
+      </c>
       <c r="BH3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BI3" t="n">
-        <v>5</v>
+        <v>339</v>
       </c>
       <c r="BJ3" t="n">
-        <v>11</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>79</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>11</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>57</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>43</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="BK3" t="inlineStr"/>
+      <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
+      <c r="BN3" t="inlineStr"/>
+      <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
       <c r="BQ3" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BR3" t="n">
         <v>0</v>
       </c>
       <c r="BS3" t="n">
-        <v>1.473684210526316</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="BT3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1186,22 +1191,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B Sai Sudharsan</t>
+          <t>HH Pandya</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sai Sudharsan</t>
+          <t>Hardik Pandya</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LHB</t>
+          <t>RHB</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RALB</t>
+          <t>RAFM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1211,163 +1216,208 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Spin</t>
+          <t>Pace</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>leg-break</t>
+          <t>fast-medium</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="K4" t="n">
+        <v>181</v>
+      </c>
+      <c r="L4" t="n">
+        <v>48</v>
+      </c>
+      <c r="M4" t="n">
+        <v>48</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>125</v>
+      </c>
+      <c r="P4" t="n">
+        <v>112</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5</v>
+      </c>
+      <c r="R4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S4" t="n">
+        <v>23</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" t="n">
+        <v>8</v>
+      </c>
+      <c r="V4" t="n">
+        <v>16</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>102</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>129</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>77</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>52</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>HH Pandya</t>
+        </is>
+      </c>
+      <c r="AL4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>66</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AT4" t="n">
         <v>59</v>
       </c>
-      <c r="L4" t="n">
-        <v>52</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>96</v>
-      </c>
-      <c r="O4" t="n">
-        <v>81</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>21</v>
-      </c>
-      <c r="R4" t="n">
-        <v>12</v>
-      </c>
-      <c r="S4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" t="n">
-        <v>8</v>
-      </c>
-      <c r="U4" t="n">
-        <v>16</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AU4" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>B Sai Sudharsan</t>
-        </is>
-      </c>
-      <c r="AK4" t="n">
-        <v>22</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>62</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>53</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>19</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>20</v>
-      </c>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr"/>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>HH Pandya</t>
+        </is>
+      </c>
+      <c r="AW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0</v>
+      </c>
       <c r="AY4" t="inlineStr"/>
       <c r="AZ4" t="inlineStr"/>
-      <c r="BA4" t="inlineStr"/>
-      <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="inlineStr"/>
+      <c r="BA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0</v>
+      </c>
       <c r="BE4" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="BF4" t="n">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="BG4" t="n">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="BH4" t="n">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="BI4" t="n">
-        <v>5</v>
-      </c>
-      <c r="BJ4" t="inlineStr"/>
-      <c r="BK4" t="inlineStr"/>
-      <c r="BL4" t="inlineStr"/>
-      <c r="BM4" t="inlineStr"/>
-      <c r="BN4" t="inlineStr"/>
-      <c r="BO4" t="inlineStr"/>
+        <v>213</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>59</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>41</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>100</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0</v>
+      </c>
       <c r="BP4" t="n">
         <v>0</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BR4" t="n">
-        <v>35.2</v>
-      </c>
-      <c r="BS4" t="inlineStr"/>
+        <v>17</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>27</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1392,7 +1442,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>RAOB</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1407,57 +1457,57 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>leg-break</t>
+          <t>off-break</t>
         </is>
       </c>
       <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" t="n">
         <v>5</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>122</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
       <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>1</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
         <v>97</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>66</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>1</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>83</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>59</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>3</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>16</v>
       </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
       <c r="V5" t="n">
         <v>0</v>
       </c>
       <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
         <v>-2</v>
       </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
       <c r="Y5" t="n">
         <v>0</v>
       </c>
@@ -1488,42 +1538,44 @@
       <c r="AH5" t="n">
         <v>0</v>
       </c>
-      <c r="AI5" t="inlineStr">
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AJ5" t="inlineStr">
+      <c r="AK5" t="inlineStr">
         <is>
           <t>DA Miller</t>
         </is>
       </c>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="n">
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="n">
         <v>31</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AN5" t="n">
         <v>2</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AO5" t="n">
         <v>17</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="AP5" t="n">
         <v>46</v>
       </c>
-      <c r="AP5" t="n">
+      <c r="AQ5" t="n">
         <v>6</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AR5" t="n">
         <v>46</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AS5" t="n">
         <v>32</v>
       </c>
-      <c r="AS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT5" t="inlineStr"/>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
       <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
@@ -1534,37 +1586,38 @@
       <c r="BB5" t="inlineStr"/>
       <c r="BC5" t="inlineStr"/>
       <c r="BD5" t="inlineStr"/>
-      <c r="BE5" t="n">
-        <v>0</v>
-      </c>
+      <c r="BE5" t="inlineStr"/>
       <c r="BF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG5" t="n">
         <v>54</v>
       </c>
-      <c r="BG5" t="n">
+      <c r="BH5" t="n">
         <v>46</v>
       </c>
-      <c r="BH5" t="n">
+      <c r="BI5" t="n">
         <v>180</v>
       </c>
-      <c r="BI5" t="n">
+      <c r="BJ5" t="n">
         <v>8</v>
       </c>
-      <c r="BJ5" t="inlineStr"/>
       <c r="BK5" t="inlineStr"/>
       <c r="BL5" t="inlineStr"/>
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="inlineStr"/>
-      <c r="BP5" t="n">
-        <v>0</v>
-      </c>
+      <c r="BP5" t="inlineStr"/>
       <c r="BQ5" t="n">
         <v>0</v>
       </c>
       <c r="BR5" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="BS5" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>22</v>
+      </c>
+      <c r="BT5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1574,12 +1627,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HH Pandya</t>
+          <t>V Shankar</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hardik Pandya</t>
+          <t>Vijay Shankar</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1589,7 +1642,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RAFM</t>
+          <t>RAM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1604,200 +1657,165 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>fast-medium</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6" t="n">
-        <v>181</v>
+        <v>4</v>
       </c>
       <c r="K6" t="n">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="L6" t="n">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="M6" t="n">
+        <v>10</v>
+      </c>
+      <c r="N6" t="n">
         <v>1</v>
-      </c>
-      <c r="N6" t="n">
-        <v>125</v>
       </c>
       <c r="O6" t="n">
         <v>112</v>
       </c>
       <c r="P6" t="n">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="Q6" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="R6" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="S6" t="n">
+        <v>31</v>
+      </c>
+      <c r="T6" t="n">
         <v>1</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>8</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>16</v>
       </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
       <c r="W6" t="n">
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>V Shankar</t>
+        </is>
+      </c>
+      <c r="AL6" t="n">
+        <v>27</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>63</v>
+      </c>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="n">
         <v>10</v>
       </c>
-      <c r="AA6" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>77</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>52</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>HH Pandya</t>
-        </is>
-      </c>
-      <c r="AK6" t="n">
-        <v>8</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>5</v>
-      </c>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="n">
-        <v>8</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>28</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>66</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>13</v>
-      </c>
       <c r="AR6" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="AS6" t="n">
-        <v>59</v>
-      </c>
-      <c r="AT6" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>HH Pandya</t>
-        </is>
-      </c>
-      <c r="AV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
       <c r="AX6" t="inlineStr"/>
       <c r="AY6" t="inlineStr"/>
-      <c r="AZ6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>23</v>
-      </c>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
+      <c r="BD6" t="inlineStr"/>
+      <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="n">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="BG6" t="n">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="BH6" t="n">
-        <v>213</v>
+        <v>42</v>
       </c>
       <c r="BI6" t="n">
-        <v>8</v>
+        <v>205</v>
       </c>
       <c r="BJ6" t="n">
-        <v>59</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>41</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>100</v>
-      </c>
-      <c r="BN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP6" t="n">
-        <v>3</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="BK6" t="inlineStr"/>
+      <c r="BL6" t="inlineStr"/>
+      <c r="BM6" t="inlineStr"/>
+      <c r="BN6" t="inlineStr"/>
+      <c r="BO6" t="inlineStr"/>
+      <c r="BP6" t="inlineStr"/>
       <c r="BQ6" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="BR6" t="n">
-        <v>26.625</v>
+        <v>0</v>
       </c>
       <c r="BS6" t="n">
-        <v>0.7058823529411765</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="BT6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1807,45 +1825,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>J Little</t>
+          <t>Rashid Khan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Joshua Little</t>
+          <t>Rashid Khan</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LHB</t>
+          <t>RHB</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LAF</t>
+          <t>RALB</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pace</t>
+          <t>Spin</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>fast</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
+          <t>leg-break</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>6</v>
+      </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -1866,13 +1886,13 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" t="n">
         <v>0</v>
@@ -1884,75 +1904,95 @@
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="Z7" t="n">
+        <v>306</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>38</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>206</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>62</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>Rashid Khan</t>
+        </is>
+      </c>
+      <c r="AL7" t="n">
         <v>10</v>
       </c>
-      <c r="AA7" t="n">
-        <v>8</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>7</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>71</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>62</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>75</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="inlineStr"/>
       <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="inlineStr"/>
+      <c r="AP7" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="inlineStr"/>
+      <c r="AR7" t="n">
+        <v>2</v>
+      </c>
       <c r="AS7" t="inlineStr"/>
-      <c r="AT7" t="inlineStr">
+      <c r="AT7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU7" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>J Little</t>
-        </is>
-      </c>
-      <c r="AV7" t="n">
-        <v>1</v>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>Rashid Khan</t>
+        </is>
       </c>
       <c r="AW7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AY7" t="n">
         <v>3</v>
       </c>
-      <c r="AZ7" t="inlineStr"/>
-      <c r="BA7" t="inlineStr"/>
+      <c r="AZ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>2</v>
+      </c>
       <c r="BB7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC7" t="n">
         <v>2</v>
@@ -1960,44 +2000,53 @@
       <c r="BD7" t="n">
         <v>0</v>
       </c>
-      <c r="BE7" t="inlineStr"/>
-      <c r="BF7" t="inlineStr"/>
-      <c r="BG7" t="inlineStr"/>
+      <c r="BE7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0</v>
+      </c>
       <c r="BH7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="BI7" t="n">
+        <v>16</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>9</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>11</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>69</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>19</v>
+      </c>
+      <c r="BN7" t="n">
         <v>7</v>
       </c>
-      <c r="BJ7" t="n">
+      <c r="BO7" t="n">
+        <v>53</v>
+      </c>
+      <c r="BP7" t="n">
         <v>40</v>
       </c>
-      <c r="BK7" t="n">
-        <v>32</v>
-      </c>
-      <c r="BL7" t="n">
-        <v>28</v>
-      </c>
-      <c r="BM7" t="n">
-        <v>29</v>
-      </c>
-      <c r="BN7" t="n">
-        <v>43</v>
-      </c>
-      <c r="BO7" t="n">
-        <v>29</v>
-      </c>
-      <c r="BP7" t="n">
-        <v>7</v>
-      </c>
       <c r="BQ7" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="BR7" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="BS7" t="n">
-        <v>1.12</v>
+        <v>2</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="8">
@@ -2008,22 +2057,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>J Yadav</t>
+          <t>R Tewatia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Jayant Yadav</t>
+          <t>Rahul Tewatia</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>RHB</t>
+          <t>LHB</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>RALB</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2038,15 +2087,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>off-break</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
+          <t>leg-break</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>7</v>
+      </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -2058,22 +2109,22 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -2085,28 +2136,28 @@
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Z8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AA8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AF8" t="n">
         <v>0</v>
@@ -2117,69 +2168,98 @@
       <c r="AH8" t="n">
         <v>0</v>
       </c>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="inlineStr"/>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>R Tewatia</t>
+        </is>
+      </c>
+      <c r="AL8" t="n">
+        <v>15</v>
+      </c>
       <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="inlineStr"/>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="inlineStr"/>
-      <c r="AQ8" t="inlineStr"/>
-      <c r="AR8" t="inlineStr"/>
+      <c r="AO8" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>20</v>
+      </c>
       <c r="AS8" t="inlineStr"/>
-      <c r="AT8" t="inlineStr">
+      <c r="AT8" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU8" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>J Yadav</t>
-        </is>
-      </c>
-      <c r="AV8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>R Tewatia</t>
+        </is>
+      </c>
       <c r="AW8" t="inlineStr"/>
       <c r="AX8" t="inlineStr"/>
       <c r="AY8" t="inlineStr"/>
       <c r="AZ8" t="inlineStr"/>
-      <c r="BA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="n">
+        <v>0</v>
+      </c>
       <c r="BC8" t="inlineStr"/>
       <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="inlineStr"/>
-      <c r="BF8" t="inlineStr"/>
-      <c r="BG8" t="inlineStr"/>
+      <c r="BF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>2</v>
+      </c>
       <c r="BH8" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="BI8" t="n">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="BJ8" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="BK8" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="BL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM8" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0</v>
+      </c>
       <c r="BN8" t="inlineStr"/>
       <c r="BO8" t="inlineStr"/>
-      <c r="BP8" t="n">
-        <v>0</v>
-      </c>
+      <c r="BP8" t="inlineStr"/>
       <c r="BQ8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BR8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS8" t="n">
+        <v>10</v>
+      </c>
+      <c r="BT8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2191,12 +2271,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MM Sharma</t>
+          <t>A Manohar</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mohit Sharma</t>
+          <t>Abhinav Manohar</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2206,7 +2286,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RAFM</t>
+          <t>RALB</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2216,20 +2296,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pace</t>
+          <t>Spin</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>fast-medium</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
+          <t>leg-break</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>8</v>
+      </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -2241,25 +2323,25 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
@@ -2268,119 +2350,112 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AC9" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="AF9" t="n">
         <v>0</v>
       </c>
       <c r="AG9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>9</v>
-      </c>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>A Manohar</t>
+        </is>
+      </c>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr"/>
+      <c r="AN9" t="n">
+        <v>14</v>
+      </c>
       <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="inlineStr"/>
-      <c r="AQ9" t="inlineStr"/>
-      <c r="AR9" t="inlineStr"/>
+      <c r="AP9" t="n">
+        <v>27</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>42</v>
+      </c>
       <c r="AS9" t="inlineStr"/>
-      <c r="AT9" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AU9" t="inlineStr">
-        <is>
-          <t>MM Sharma</t>
-        </is>
-      </c>
+      <c r="AT9" t="n">
+        <v>26</v>
+      </c>
+      <c r="AU9" t="inlineStr"/>
       <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="inlineStr"/>
       <c r="AX9" t="inlineStr"/>
-      <c r="AY9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AZ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA9" t="n">
-        <v>4</v>
-      </c>
-      <c r="BB9" t="n">
-        <v>3</v>
-      </c>
-      <c r="BC9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD9" t="n">
-        <v>2</v>
-      </c>
+      <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
+      <c r="BB9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
+      <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
-      <c r="BF9" t="inlineStr"/>
-      <c r="BG9" t="inlineStr"/>
+      <c r="BF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>57</v>
+      </c>
       <c r="BH9" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="BI9" t="n">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="BJ9" t="n">
-        <v>6</v>
-      </c>
-      <c r="BK9" t="n">
-        <v>56</v>
-      </c>
-      <c r="BL9" t="n">
-        <v>39</v>
-      </c>
-      <c r="BM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN9" t="n">
-        <v>18</v>
-      </c>
-      <c r="BO9" t="n">
-        <v>82</v>
-      </c>
-      <c r="BP9" t="n">
-        <v>11</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BK9" t="inlineStr"/>
+      <c r="BL9" t="inlineStr"/>
+      <c r="BM9" t="inlineStr"/>
+      <c r="BN9" t="inlineStr"/>
+      <c r="BO9" t="inlineStr"/>
+      <c r="BP9" t="inlineStr"/>
       <c r="BQ9" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BR9" t="n">
         <v>0</v>
       </c>
       <c r="BS9" t="n">
-        <v>2.444444444444445</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="BT9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2390,12 +2465,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mohammed Shami</t>
+          <t>MM Sharma</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Mohammed Shami</t>
+          <t>Mohit Sharma</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2423,10 +2498,10 @@
           <t>fast-medium</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
+      <c r="I10" t="n">
+        <v>9</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>0</v>
       </c>
@@ -2467,39 +2542,41 @@
         <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>233</v>
+        <v>108</v>
       </c>
       <c r="Z10" t="n">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="AA10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>75</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>43</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="n">
         <v>2</v>
       </c>
-      <c r="AB10" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>139</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>14</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>80</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>12</v>
-      </c>
-      <c r="AG10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH10" t="n">
-        <v>5</v>
-      </c>
-      <c r="AI10" t="inlineStr"/>
+      <c r="AI10" t="n">
+        <v>9</v>
+      </c>
       <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr"/>
@@ -2510,81 +2587,76 @@
       <c r="AQ10" t="inlineStr"/>
       <c r="AR10" t="inlineStr"/>
       <c r="AS10" t="inlineStr"/>
-      <c r="AT10" t="inlineStr">
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AU10" t="inlineStr">
-        <is>
-          <t>Mohammed Shami</t>
-        </is>
-      </c>
-      <c r="AV10" t="n">
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>MM Sharma</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr"/>
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" t="n">
         <v>2</v>
       </c>
-      <c r="AW10" t="n">
-        <v>3</v>
-      </c>
-      <c r="AX10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ10" t="n">
-        <v>3</v>
-      </c>
       <c r="BA10" t="n">
         <v>0</v>
       </c>
       <c r="BB10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BC10" t="n">
         <v>3</v>
       </c>
       <c r="BD10" t="n">
-        <v>4</v>
-      </c>
-      <c r="BE10" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>2</v>
+      </c>
       <c r="BF10" t="inlineStr"/>
       <c r="BG10" t="inlineStr"/>
-      <c r="BH10" t="n">
-        <v>0</v>
-      </c>
+      <c r="BH10" t="inlineStr"/>
       <c r="BI10" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BJ10" t="n">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="BK10" t="n">
         <v>6</v>
       </c>
       <c r="BL10" t="n">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="BM10" t="n">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="BN10" t="n">
         <v>0</v>
       </c>
       <c r="BO10" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="BP10" t="n">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="BQ10" t="n">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="BR10" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="BS10" t="n">
-        <v>1.942857142857143</v>
+        <v>0</v>
+      </c>
+      <c r="BT10" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="11">
@@ -2595,12 +2667,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Noor Ahmad</t>
+          <t>Mohammed Shami</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Noor Ahmad</t>
+          <t>Mohammed Shami</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2610,28 +2682,28 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LACM</t>
+          <t>RAFM</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Spin</t>
+          <t>Pace</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>chinaman</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
+          <t>fast-medium</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
         <v>0</v>
       </c>
@@ -2672,39 +2744,41 @@
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="Y11" t="n">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>233</v>
       </c>
       <c r="AA11" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AB11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC11" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD11" t="n">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="AE11" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AG11" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AH11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI11" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>5</v>
+      </c>
       <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
@@ -2715,73 +2789,82 @@
       <c r="AQ11" t="inlineStr"/>
       <c r="AR11" t="inlineStr"/>
       <c r="AS11" t="inlineStr"/>
-      <c r="AT11" t="inlineStr">
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AU11" t="inlineStr">
-        <is>
-          <t>Noor Ahmad</t>
-        </is>
-      </c>
-      <c r="AV11" t="inlineStr"/>
-      <c r="AW11" t="inlineStr"/>
-      <c r="AX11" t="inlineStr"/>
-      <c r="AY11" t="inlineStr"/>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>Mohammed Shami</t>
+        </is>
+      </c>
+      <c r="AW11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>1</v>
+      </c>
       <c r="AZ11" t="n">
         <v>1</v>
       </c>
       <c r="BA11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD11" t="n">
         <v>3</v>
       </c>
-      <c r="BC11" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD11" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE11" t="inlineStr"/>
+      <c r="BE11" t="n">
+        <v>4</v>
+      </c>
       <c r="BF11" t="inlineStr"/>
       <c r="BG11" t="inlineStr"/>
-      <c r="BH11" t="n">
-        <v>0</v>
-      </c>
+      <c r="BH11" t="inlineStr"/>
       <c r="BI11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BJ11" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BK11" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="BL11" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="BM11" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="BN11" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="BO11" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="BP11" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="BQ11" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="BR11" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="BS11" t="n">
-        <v>1.684210526315789</v>
+        <v>0</v>
+      </c>
+      <c r="BT11" t="n">
+        <v>1.9</v>
       </c>
     </row>
     <row r="12">
@@ -2792,27 +2875,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R Tewatia</t>
+          <t>Noor Ahmad</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Rahul Tewatia</t>
+          <t>Noor Ahmad</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>LHB</t>
+          <t>RHB</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RALB</t>
+          <t>LACM</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2822,177 +2905,166 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>leg-break</t>
+          <t>chinaman</t>
         </is>
       </c>
       <c r="I12" t="n">
+        <v>11</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>110</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>121</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="n">
         <v>6</v>
       </c>
-      <c r="J12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" t="n">
-        <v>3</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>62</v>
-      </c>
-      <c r="R12" t="n">
-        <v>30</v>
-      </c>
-      <c r="S12" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>7</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI12" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AJ12" t="inlineStr">
-        <is>
-          <t>R Tewatia</t>
-        </is>
-      </c>
-      <c r="AK12" t="n">
-        <v>15</v>
-      </c>
+      <c r="AI12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
-      <c r="AN12" t="n">
-        <v>5</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ12" t="n">
-        <v>20</v>
-      </c>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
       <c r="AR12" t="inlineStr"/>
-      <c r="AS12" t="n">
-        <v>20</v>
-      </c>
-      <c r="AT12" t="inlineStr">
+      <c r="AS12" t="inlineStr"/>
+      <c r="AT12" t="inlineStr"/>
+      <c r="AU12" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AU12" t="inlineStr">
-        <is>
-          <t>R Tewatia</t>
-        </is>
-      </c>
-      <c r="AV12" t="inlineStr"/>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>Noor Ahmad</t>
+        </is>
+      </c>
       <c r="AW12" t="inlineStr"/>
       <c r="AX12" t="inlineStr"/>
       <c r="AY12" t="inlineStr"/>
       <c r="AZ12" t="inlineStr"/>
       <c r="BA12" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB12" t="inlineStr"/>
-      <c r="BC12" t="inlineStr"/>
-      <c r="BD12" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>2</v>
+      </c>
       <c r="BE12" t="n">
         <v>0</v>
       </c>
-      <c r="BF12" t="n">
-        <v>2</v>
-      </c>
-      <c r="BG12" t="n">
-        <v>98</v>
-      </c>
-      <c r="BH12" t="n">
-        <v>63</v>
-      </c>
+      <c r="BF12" t="inlineStr"/>
+      <c r="BG12" t="inlineStr"/>
+      <c r="BH12" t="inlineStr"/>
       <c r="BI12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BJ12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BK12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="BL12" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM12" t="inlineStr"/>
-      <c r="BN12" t="inlineStr"/>
-      <c r="BO12" t="inlineStr"/>
+        <v>79</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>21</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO12" t="n">
+        <v>75</v>
+      </c>
       <c r="BP12" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="BQ12" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="BR12" t="n">
-        <v>10.5</v>
+        <v>19</v>
       </c>
       <c r="BS12" t="n">
         <v>0</v>
+      </c>
+      <c r="BT12" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="13">
@@ -3003,12 +3075,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rashid Khan</t>
+          <t>AS Joseph</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Rashid Khan</t>
+          <t>Alzarri Joseph</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3018,7 +3090,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RALB</t>
+          <t>RAFM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3028,20 +3100,18 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Spin</t>
+          <t>Pace</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>leg-break</t>
+          <t>fast-medium</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>7</v>
-      </c>
-      <c r="J13" t="n">
-        <v>7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>0</v>
       </c>
@@ -3061,13 +3131,13 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
@@ -3082,146 +3152,119 @@
         <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>216</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="n">
-        <v>306</v>
+        <v>114</v>
       </c>
       <c r="Z13" t="n">
+        <v>162</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>15</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>133</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="n">
         <v>4</v>
       </c>
-      <c r="AA13" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>7</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>38</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>206</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>62</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>8</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>6</v>
-      </c>
-      <c r="AI13" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AJ13" t="inlineStr">
-        <is>
-          <t>Rashid Khan</t>
-        </is>
-      </c>
-      <c r="AK13" t="n">
-        <v>10</v>
-      </c>
+      <c r="AI13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="n">
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>AS Joseph</t>
+        </is>
+      </c>
+      <c r="AW13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ13" t="n">
         <v>1</v>
       </c>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR13" t="inlineStr"/>
-      <c r="AS13" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT13" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AU13" t="inlineStr">
-        <is>
-          <t>Rashid Khan</t>
-        </is>
-      </c>
-      <c r="AV13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW13" t="n">
-        <v>3</v>
-      </c>
-      <c r="AX13" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ13" t="n">
-        <v>2</v>
-      </c>
       <c r="BA13" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB13" t="n">
-        <v>2</v>
-      </c>
-      <c r="BC13" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD13" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE13" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF13" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG13" t="n">
-        <v>100</v>
-      </c>
-      <c r="BH13" t="n">
-        <v>16</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="BB13" t="inlineStr"/>
+      <c r="BC13" t="inlineStr"/>
+      <c r="BD13" t="inlineStr"/>
+      <c r="BE13" t="inlineStr"/>
+      <c r="BF13" t="inlineStr"/>
+      <c r="BG13" t="inlineStr"/>
+      <c r="BH13" t="inlineStr"/>
       <c r="BI13" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BJ13" t="n">
+        <v>5</v>
+      </c>
+      <c r="BK13" t="n">
         <v>11</v>
       </c>
-      <c r="BK13" t="n">
-        <v>69</v>
-      </c>
       <c r="BL13" t="n">
+        <v>79</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>11</v>
+      </c>
+      <c r="BN13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO13" t="n">
+        <v>57</v>
+      </c>
+      <c r="BP13" t="n">
+        <v>43</v>
+      </c>
+      <c r="BQ13" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR13" t="n">
         <v>19</v>
       </c>
-      <c r="BM13" t="n">
-        <v>7</v>
-      </c>
-      <c r="BN13" t="n">
-        <v>53</v>
-      </c>
-      <c r="BO13" t="n">
-        <v>40</v>
-      </c>
-      <c r="BP13" t="n">
-        <v>15</v>
-      </c>
-      <c r="BQ13" t="n">
-        <v>36</v>
-      </c>
-      <c r="BR13" t="n">
-        <v>1.777777777777778</v>
-      </c>
       <c r="BS13" t="n">
-        <v>1.666666666666667</v>
+        <v>0</v>
+      </c>
+      <c r="BT13" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="14">
@@ -3232,196 +3275,199 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Shubman Gill</t>
+          <t>J Little</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Shubman Gill</t>
+          <t>Joshua Little</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>RHB</t>
+          <t>LHB</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>LAF</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Spin</t>
+          <t>Pace</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>off-break</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
+          <t>fast</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>150</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>208</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>71</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>62</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>75</v>
+      </c>
+      <c r="AG14" t="n">
         <v>2</v>
       </c>
-      <c r="J14" t="n">
-        <v>240</v>
-      </c>
-      <c r="K14" t="n">
-        <v>166</v>
-      </c>
-      <c r="L14" t="n">
-        <v>115</v>
-      </c>
-      <c r="M14" t="n">
-        <v>4</v>
-      </c>
-      <c r="N14" t="n">
-        <v>158</v>
-      </c>
-      <c r="O14" t="n">
-        <v>123</v>
-      </c>
-      <c r="P14" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>15</v>
-      </c>
-      <c r="R14" t="n">
-        <v>8</v>
-      </c>
-      <c r="S14" t="n">
+      <c r="AH14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
+      <c r="AU14" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>J Little</t>
+        </is>
+      </c>
+      <c r="AW14" t="n">
         <v>1</v>
       </c>
-      <c r="T14" t="n">
-        <v>24</v>
-      </c>
-      <c r="U14" t="n">
-        <v>24</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
-      <c r="W14" t="n">
-        <v>-2</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI14" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="AJ14" t="inlineStr">
-        <is>
-          <t>Shubman Gill</t>
-        </is>
-      </c>
-      <c r="AK14" t="n">
-        <v>63</v>
-      </c>
-      <c r="AL14" t="n">
-        <v>14</v>
-      </c>
-      <c r="AM14" t="n">
-        <v>39</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>67</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>45</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>56</v>
-      </c>
-      <c r="AR14" t="n">
-        <v>49</v>
-      </c>
-      <c r="AS14" t="n">
-        <v>6</v>
-      </c>
-      <c r="AT14" t="inlineStr"/>
-      <c r="AU14" t="inlineStr"/>
-      <c r="AV14" t="inlineStr"/>
-      <c r="AW14" t="inlineStr"/>
-      <c r="AX14" t="inlineStr"/>
-      <c r="AY14" t="inlineStr"/>
-      <c r="AZ14" t="inlineStr"/>
+      <c r="AX14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>3</v>
+      </c>
       <c r="BA14" t="inlineStr"/>
       <c r="BB14" t="inlineStr"/>
-      <c r="BC14" t="inlineStr"/>
-      <c r="BD14" t="inlineStr"/>
+      <c r="BC14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>2</v>
+      </c>
       <c r="BE14" t="n">
-        <v>49</v>
-      </c>
-      <c r="BF14" t="n">
-        <v>47</v>
-      </c>
-      <c r="BG14" t="n">
-        <v>4</v>
-      </c>
-      <c r="BH14" t="n">
-        <v>339</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="BF14" t="inlineStr"/>
+      <c r="BG14" t="inlineStr"/>
+      <c r="BH14" t="inlineStr"/>
       <c r="BI14" t="n">
-        <v>9</v>
-      </c>
-      <c r="BJ14" t="inlineStr"/>
-      <c r="BK14" t="inlineStr"/>
-      <c r="BL14" t="inlineStr"/>
-      <c r="BM14" t="inlineStr"/>
-      <c r="BN14" t="inlineStr"/>
-      <c r="BO14" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>7</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>40</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>32</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>28</v>
+      </c>
+      <c r="BN14" t="n">
+        <v>29</v>
+      </c>
+      <c r="BO14" t="n">
+        <v>43</v>
+      </c>
       <c r="BP14" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="BQ14" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BR14" t="n">
-        <v>37.66666666666666</v>
-      </c>
-      <c r="BS14" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="BS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT14" t="n">
+        <v>1.1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3431,22 +3477,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>V Shankar</t>
+          <t>B Sai Sudharsan</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Vijay Shankar</t>
+          <t>Sai Sudharsan</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>RHB</t>
+          <t>LHB</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>RAM</t>
+          <t>RALB</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -3456,56 +3502,54 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Pace</t>
+          <t>Spin</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>4</v>
-      </c>
+          <t>leg-break</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="n">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="K15" t="n">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="L15" t="n">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="M15" t="n">
+        <v>52</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>96</v>
+      </c>
+      <c r="P15" t="n">
+        <v>81</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" t="n">
+        <v>21</v>
+      </c>
+      <c r="S15" t="n">
+        <v>12</v>
+      </c>
+      <c r="T15" t="n">
         <v>1</v>
       </c>
-      <c r="N15" t="n">
-        <v>112</v>
-      </c>
-      <c r="O15" t="n">
-        <v>95</v>
-      </c>
-      <c r="P15" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>87</v>
-      </c>
-      <c r="R15" t="n">
-        <v>31</v>
-      </c>
-      <c r="S15" t="n">
-        <v>1</v>
-      </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>8</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>16</v>
       </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
       <c r="W15" t="n">
         <v>0</v>
       </c>
@@ -3542,39 +3586,37 @@
       <c r="AH15" t="n">
         <v>0</v>
       </c>
-      <c r="AI15" t="inlineStr">
+      <c r="AI15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AJ15" t="inlineStr">
-        <is>
-          <t>V Shankar</t>
-        </is>
-      </c>
-      <c r="AK15" t="n">
-        <v>27</v>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>B Sai Sudharsan</t>
+        </is>
       </c>
       <c r="AL15" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="AM15" t="n">
-        <v>63</v>
-      </c>
-      <c r="AN15" t="inlineStr"/>
-      <c r="AO15" t="inlineStr"/>
+        <v>62</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>53</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>19</v>
+      </c>
       <c r="AP15" t="n">
-        <v>10</v>
-      </c>
-      <c r="AQ15" t="n">
-        <v>19</v>
-      </c>
-      <c r="AR15" t="n">
-        <v>51</v>
-      </c>
-      <c r="AS15" t="n">
-        <v>6</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
       <c r="AT15" t="inlineStr"/>
       <c r="AU15" t="inlineStr"/>
       <c r="AV15" t="inlineStr"/>
@@ -3586,37 +3628,38 @@
       <c r="BB15" t="inlineStr"/>
       <c r="BC15" t="inlineStr"/>
       <c r="BD15" t="inlineStr"/>
-      <c r="BE15" t="n">
-        <v>3</v>
-      </c>
+      <c r="BE15" t="inlineStr"/>
       <c r="BF15" t="n">
+        <v>34</v>
+      </c>
+      <c r="BG15" t="n">
         <v>55</v>
       </c>
-      <c r="BG15" t="n">
-        <v>42</v>
-      </c>
       <c r="BH15" t="n">
-        <v>205</v>
+        <v>12</v>
       </c>
       <c r="BI15" t="n">
-        <v>7</v>
-      </c>
-      <c r="BJ15" t="inlineStr"/>
+        <v>176</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>5</v>
+      </c>
       <c r="BK15" t="inlineStr"/>
       <c r="BL15" t="inlineStr"/>
       <c r="BM15" t="inlineStr"/>
       <c r="BN15" t="inlineStr"/>
       <c r="BO15" t="inlineStr"/>
-      <c r="BP15" t="n">
-        <v>0</v>
-      </c>
+      <c r="BP15" t="inlineStr"/>
       <c r="BQ15" t="n">
         <v>0</v>
       </c>
       <c r="BR15" t="n">
-        <v>29.28571428571428</v>
-      </c>
-      <c r="BS15" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="BS15" t="n">
+        <v>35</v>
+      </c>
+      <c r="BT15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3626,94 +3669,106 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WP Saha</t>
+          <t>Yash Dayal</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wriddhiman Saha</t>
+          <t>Yash Dayal</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>RHB</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
+          <t>LHB</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LAFM</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Pace</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>fast-medium</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>36</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>95</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC16" t="n">
         <v>1</v>
       </c>
-      <c r="J16" t="n">
-        <v>121</v>
-      </c>
-      <c r="K16" t="n">
-        <v>138</v>
-      </c>
-      <c r="L16" t="n">
-        <v>114</v>
-      </c>
-      <c r="M16" t="n">
-        <v>8</v>
-      </c>
-      <c r="N16" t="n">
-        <v>13</v>
-      </c>
-      <c r="O16" t="n">
-        <v>13</v>
-      </c>
-      <c r="P16" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>8</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>-2</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0</v>
-      </c>
       <c r="AD16" t="n">
         <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="AF16" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AG16" t="n">
         <v>0</v>
@@ -3721,85 +3776,78 @@
       <c r="AH16" t="n">
         <v>0</v>
       </c>
-      <c r="AI16" t="inlineStr">
+      <c r="AI16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AJ16" t="inlineStr">
-        <is>
-          <t>WP Saha</t>
-        </is>
-      </c>
-      <c r="AK16" t="n">
-        <v>25</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>14</v>
-      </c>
-      <c r="AM16" t="n">
-        <v>17</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>30</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>4</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>47</v>
-      </c>
-      <c r="AQ16" t="n">
-        <v>4</v>
-      </c>
-      <c r="AR16" t="n">
-        <v>10</v>
-      </c>
-      <c r="AS16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="inlineStr"/>
-      <c r="AV16" t="inlineStr"/>
-      <c r="AW16" t="inlineStr"/>
-      <c r="AX16" t="inlineStr"/>
-      <c r="AY16" t="inlineStr"/>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>Yash Dayal</t>
+        </is>
+      </c>
+      <c r="AW16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY16" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ16" t="inlineStr"/>
       <c r="BA16" t="inlineStr"/>
       <c r="BB16" t="inlineStr"/>
       <c r="BC16" t="inlineStr"/>
       <c r="BD16" t="inlineStr"/>
-      <c r="BE16" t="n">
-        <v>91</v>
-      </c>
-      <c r="BF16" t="n">
-        <v>9</v>
-      </c>
-      <c r="BG16" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH16" t="n">
-        <v>151</v>
-      </c>
+      <c r="BE16" t="inlineStr"/>
+      <c r="BF16" t="inlineStr"/>
+      <c r="BG16" t="inlineStr"/>
+      <c r="BH16" t="inlineStr"/>
       <c r="BI16" t="n">
-        <v>9</v>
-      </c>
-      <c r="BJ16" t="inlineStr"/>
-      <c r="BK16" t="inlineStr"/>
-      <c r="BL16" t="inlineStr"/>
-      <c r="BM16" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>3</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>83</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>17</v>
+      </c>
       <c r="BN16" t="inlineStr"/>
       <c r="BO16" t="inlineStr"/>
-      <c r="BP16" t="n">
-        <v>0</v>
-      </c>
+      <c r="BP16" t="inlineStr"/>
       <c r="BQ16" t="n">
         <v>0</v>
       </c>
       <c r="BR16" t="n">
-        <v>16.77777777777778</v>
-      </c>
-      <c r="BS16" t="inlineStr"/>
+        <v>6</v>
+      </c>
+      <c r="BS16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3809,43 +3857,41 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Yash Dayal</t>
+          <t>J Yadav</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Yash Dayal</t>
+          <t>Jayant Yadav</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>LHB</t>
+          <t>RHB</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LAFM</t>
+          <t>RAOB</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pace</t>
+          <t>Spin</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>fast-medium</t>
+          <t>off-break</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
         <v>0</v>
       </c>
@@ -3886,28 +3932,28 @@
         <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="Y17" t="n">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AA17" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AB17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC17" t="n">
         <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="AE17" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="AF17" t="n">
         <v>0</v>
@@ -3918,7 +3964,9 @@
       <c r="AH17" t="n">
         <v>0</v>
       </c>
-      <c r="AI17" t="inlineStr"/>
+      <c r="AI17" t="n">
+        <v>0</v>
+      </c>
       <c r="AJ17" t="inlineStr"/>
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr"/>
@@ -3929,62 +3977,59 @@
       <c r="AQ17" t="inlineStr"/>
       <c r="AR17" t="inlineStr"/>
       <c r="AS17" t="inlineStr"/>
-      <c r="AT17" t="inlineStr">
+      <c r="AT17" t="inlineStr"/>
+      <c r="AU17" t="inlineStr">
         <is>
           <t>Gujarat Titans</t>
         </is>
       </c>
-      <c r="AU17" t="inlineStr">
-        <is>
-          <t>Yash Dayal</t>
-        </is>
-      </c>
-      <c r="AV17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX17" t="n">
-        <v>0</v>
-      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>J Yadav</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr"/>
+      <c r="AX17" t="inlineStr"/>
       <c r="AY17" t="inlineStr"/>
       <c r="AZ17" t="inlineStr"/>
       <c r="BA17" t="inlineStr"/>
-      <c r="BB17" t="inlineStr"/>
+      <c r="BB17" t="n">
+        <v>0</v>
+      </c>
       <c r="BC17" t="inlineStr"/>
       <c r="BD17" t="inlineStr"/>
       <c r="BE17" t="inlineStr"/>
       <c r="BF17" t="inlineStr"/>
       <c r="BG17" t="inlineStr"/>
-      <c r="BH17" t="n">
-        <v>0</v>
-      </c>
+      <c r="BH17" t="inlineStr"/>
       <c r="BI17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BJ17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK17" t="n">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="BL17" t="n">
-        <v>17</v>
-      </c>
-      <c r="BM17" t="inlineStr"/>
+        <v>50</v>
+      </c>
+      <c r="BM17" t="n">
+        <v>0</v>
+      </c>
       <c r="BN17" t="inlineStr"/>
       <c r="BO17" t="inlineStr"/>
-      <c r="BP17" t="n">
-        <v>0</v>
-      </c>
+      <c r="BP17" t="inlineStr"/>
       <c r="BQ17" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BR17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BS17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>